<commit_message>
Fix missing view change methods
</commit_message>
<xml_diff>
--- a/data/market_stats_2025-12.xlsx
+++ b/data/market_stats_2025-12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M997"/>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47312,6 +47312,147 @@
         <v>4</v>
       </c>
     </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>2025-12-04 20:14:05</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>2025-12-04</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>20:14:05</t>
+        </is>
+      </c>
+      <c r="D998" t="n">
+        <v>5756</v>
+      </c>
+      <c r="E998" t="n">
+        <v>1410</v>
+      </c>
+      <c r="F998" t="n">
+        <v>3641</v>
+      </c>
+      <c r="G998" t="n">
+        <v>705</v>
+      </c>
+      <c r="H998" t="n">
+        <v>253</v>
+      </c>
+      <c r="I998" t="n">
+        <v>530</v>
+      </c>
+      <c r="J998" t="n">
+        <v>124</v>
+      </c>
+      <c r="K998" t="n">
+        <v>140</v>
+      </c>
+      <c r="L998" t="n">
+        <v>44</v>
+      </c>
+      <c r="M998" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>2025-12-04 20:14:27</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>2025-12-04</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>20:14:27</t>
+        </is>
+      </c>
+      <c r="D999" t="n">
+        <v>5758</v>
+      </c>
+      <c r="E999" t="n">
+        <v>1410</v>
+      </c>
+      <c r="F999" t="n">
+        <v>3641</v>
+      </c>
+      <c r="G999" t="n">
+        <v>707</v>
+      </c>
+      <c r="H999" t="n">
+        <v>253</v>
+      </c>
+      <c r="I999" t="n">
+        <v>530</v>
+      </c>
+      <c r="J999" t="n">
+        <v>124</v>
+      </c>
+      <c r="K999" t="n">
+        <v>140</v>
+      </c>
+      <c r="L999" t="n">
+        <v>44</v>
+      </c>
+      <c r="M999" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>2025-12-04 20:14:49</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>2025-12-04</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>20:14:49</t>
+        </is>
+      </c>
+      <c r="D1000" t="n">
+        <v>5758</v>
+      </c>
+      <c r="E1000" t="n">
+        <v>1410</v>
+      </c>
+      <c r="F1000" t="n">
+        <v>3641</v>
+      </c>
+      <c r="G1000" t="n">
+        <v>707</v>
+      </c>
+      <c r="H1000" t="n">
+        <v>253</v>
+      </c>
+      <c r="I1000" t="n">
+        <v>530</v>
+      </c>
+      <c r="J1000" t="n">
+        <v>124</v>
+      </c>
+      <c r="K1000" t="n">
+        <v>140</v>
+      </c>
+      <c r="L1000" t="n">
+        <v>44</v>
+      </c>
+      <c r="M1000" t="n">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix auto-refresh for all views
</commit_message>
<xml_diff>
--- a/data/market_stats_2025-12.xlsx
+++ b/data/market_stats_2025-12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1002"/>
+  <dimension ref="A1:M1089"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47547,6 +47547,4095 @@
         <v>6</v>
       </c>
     </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:09:33</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>10:09:33</t>
+        </is>
+      </c>
+      <c r="D1003" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1003" t="n">
+        <v>1450</v>
+      </c>
+      <c r="F1003" t="n">
+        <v>3568</v>
+      </c>
+      <c r="G1003" t="n">
+        <v>747</v>
+      </c>
+      <c r="H1003" t="n">
+        <v>175</v>
+      </c>
+      <c r="I1003" t="n">
+        <v>319</v>
+      </c>
+      <c r="J1003" t="n">
+        <v>78</v>
+      </c>
+      <c r="K1003" t="n">
+        <v>88</v>
+      </c>
+      <c r="L1003" t="n">
+        <v>33</v>
+      </c>
+      <c r="M1003" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:09:43</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>10:09:43</t>
+        </is>
+      </c>
+      <c r="D1004" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1004" t="n">
+        <v>1452</v>
+      </c>
+      <c r="F1004" t="n">
+        <v>3582</v>
+      </c>
+      <c r="G1004" t="n">
+        <v>731</v>
+      </c>
+      <c r="H1004" t="n">
+        <v>174</v>
+      </c>
+      <c r="I1004" t="n">
+        <v>322</v>
+      </c>
+      <c r="J1004" t="n">
+        <v>76</v>
+      </c>
+      <c r="K1004" t="n">
+        <v>89</v>
+      </c>
+      <c r="L1004" t="n">
+        <v>33</v>
+      </c>
+      <c r="M1004" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:09:54</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>10:09:54</t>
+        </is>
+      </c>
+      <c r="D1005" t="n">
+        <v>5767</v>
+      </c>
+      <c r="E1005" t="n">
+        <v>1437</v>
+      </c>
+      <c r="F1005" t="n">
+        <v>3597</v>
+      </c>
+      <c r="G1005" t="n">
+        <v>733</v>
+      </c>
+      <c r="H1005" t="n">
+        <v>177</v>
+      </c>
+      <c r="I1005" t="n">
+        <v>321</v>
+      </c>
+      <c r="J1005" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1005" t="n">
+        <v>89</v>
+      </c>
+      <c r="L1005" t="n">
+        <v>33</v>
+      </c>
+      <c r="M1005" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:10:04</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>10:10:04</t>
+        </is>
+      </c>
+      <c r="D1006" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1006" t="n">
+        <v>1408</v>
+      </c>
+      <c r="F1006" t="n">
+        <v>3616</v>
+      </c>
+      <c r="G1006" t="n">
+        <v>740</v>
+      </c>
+      <c r="H1006" t="n">
+        <v>177</v>
+      </c>
+      <c r="I1006" t="n">
+        <v>312</v>
+      </c>
+      <c r="J1006" t="n">
+        <v>80</v>
+      </c>
+      <c r="K1006" t="n">
+        <v>86</v>
+      </c>
+      <c r="L1006" t="n">
+        <v>32</v>
+      </c>
+      <c r="M1006" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:10:13</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>10:10:13</t>
+        </is>
+      </c>
+      <c r="D1007" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1007" t="n">
+        <v>1434</v>
+      </c>
+      <c r="F1007" t="n">
+        <v>3603</v>
+      </c>
+      <c r="G1007" t="n">
+        <v>726</v>
+      </c>
+      <c r="H1007" t="n">
+        <v>178</v>
+      </c>
+      <c r="I1007" t="n">
+        <v>308</v>
+      </c>
+      <c r="J1007" t="n">
+        <v>81</v>
+      </c>
+      <c r="K1007" t="n">
+        <v>88</v>
+      </c>
+      <c r="L1007" t="n">
+        <v>32</v>
+      </c>
+      <c r="M1007" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:10:23</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>10:10:23</t>
+        </is>
+      </c>
+      <c r="D1008" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1008" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F1008" t="n">
+        <v>3618</v>
+      </c>
+      <c r="G1008" t="n">
+        <v>725</v>
+      </c>
+      <c r="H1008" t="n">
+        <v>177</v>
+      </c>
+      <c r="I1008" t="n">
+        <v>320</v>
+      </c>
+      <c r="J1008" t="n">
+        <v>82</v>
+      </c>
+      <c r="K1008" t="n">
+        <v>88</v>
+      </c>
+      <c r="L1008" t="n">
+        <v>32</v>
+      </c>
+      <c r="M1008" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:10:33</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>10:10:33</t>
+        </is>
+      </c>
+      <c r="D1009" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1009" t="n">
+        <v>1415</v>
+      </c>
+      <c r="F1009" t="n">
+        <v>3633</v>
+      </c>
+      <c r="G1009" t="n">
+        <v>717</v>
+      </c>
+      <c r="H1009" t="n">
+        <v>176</v>
+      </c>
+      <c r="I1009" t="n">
+        <v>315</v>
+      </c>
+      <c r="J1009" t="n">
+        <v>82</v>
+      </c>
+      <c r="K1009" t="n">
+        <v>89</v>
+      </c>
+      <c r="L1009" t="n">
+        <v>32</v>
+      </c>
+      <c r="M1009" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:10:43</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>10:10:43</t>
+        </is>
+      </c>
+      <c r="D1010" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1010" t="n">
+        <v>1411</v>
+      </c>
+      <c r="F1010" t="n">
+        <v>3627</v>
+      </c>
+      <c r="G1010" t="n">
+        <v>726</v>
+      </c>
+      <c r="H1010" t="n">
+        <v>181</v>
+      </c>
+      <c r="I1010" t="n">
+        <v>314</v>
+      </c>
+      <c r="J1010" t="n">
+        <v>82</v>
+      </c>
+      <c r="K1010" t="n">
+        <v>90</v>
+      </c>
+      <c r="L1010" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1010" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:10:53</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>10:10:53</t>
+        </is>
+      </c>
+      <c r="D1011" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1011" t="n">
+        <v>1415</v>
+      </c>
+      <c r="F1011" t="n">
+        <v>3612</v>
+      </c>
+      <c r="G1011" t="n">
+        <v>739</v>
+      </c>
+      <c r="H1011" t="n">
+        <v>178</v>
+      </c>
+      <c r="I1011" t="n">
+        <v>313</v>
+      </c>
+      <c r="J1011" t="n">
+        <v>81</v>
+      </c>
+      <c r="K1011" t="n">
+        <v>92</v>
+      </c>
+      <c r="L1011" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1011" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:11:04</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>10:11:04</t>
+        </is>
+      </c>
+      <c r="D1012" t="n">
+        <v>5762</v>
+      </c>
+      <c r="E1012" t="n">
+        <v>1411</v>
+      </c>
+      <c r="F1012" t="n">
+        <v>3625</v>
+      </c>
+      <c r="G1012" t="n">
+        <v>726</v>
+      </c>
+      <c r="H1012" t="n">
+        <v>178</v>
+      </c>
+      <c r="I1012" t="n">
+        <v>312</v>
+      </c>
+      <c r="J1012" t="n">
+        <v>82</v>
+      </c>
+      <c r="K1012" t="n">
+        <v>89</v>
+      </c>
+      <c r="L1012" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1012" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:11:13</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>10:11:13</t>
+        </is>
+      </c>
+      <c r="D1013" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1013" t="n">
+        <v>1421</v>
+      </c>
+      <c r="F1013" t="n">
+        <v>3610</v>
+      </c>
+      <c r="G1013" t="n">
+        <v>735</v>
+      </c>
+      <c r="H1013" t="n">
+        <v>175</v>
+      </c>
+      <c r="I1013" t="n">
+        <v>313</v>
+      </c>
+      <c r="J1013" t="n">
+        <v>81</v>
+      </c>
+      <c r="K1013" t="n">
+        <v>89</v>
+      </c>
+      <c r="L1013" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1013" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:11:23</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>10:11:23</t>
+        </is>
+      </c>
+      <c r="D1014" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1014" t="n">
+        <v>1407</v>
+      </c>
+      <c r="F1014" t="n">
+        <v>3637</v>
+      </c>
+      <c r="G1014" t="n">
+        <v>720</v>
+      </c>
+      <c r="H1014" t="n">
+        <v>171</v>
+      </c>
+      <c r="I1014" t="n">
+        <v>321</v>
+      </c>
+      <c r="J1014" t="n">
+        <v>77</v>
+      </c>
+      <c r="K1014" t="n">
+        <v>87</v>
+      </c>
+      <c r="L1014" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1014" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:11:34</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>10:11:34</t>
+        </is>
+      </c>
+      <c r="D1015" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1015" t="n">
+        <v>1401</v>
+      </c>
+      <c r="F1015" t="n">
+        <v>3629</v>
+      </c>
+      <c r="G1015" t="n">
+        <v>735</v>
+      </c>
+      <c r="H1015" t="n">
+        <v>174</v>
+      </c>
+      <c r="I1015" t="n">
+        <v>325</v>
+      </c>
+      <c r="J1015" t="n">
+        <v>77</v>
+      </c>
+      <c r="K1015" t="n">
+        <v>88</v>
+      </c>
+      <c r="L1015" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1015" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:11:44</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>10:11:44</t>
+        </is>
+      </c>
+      <c r="D1016" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1016" t="n">
+        <v>1412</v>
+      </c>
+      <c r="F1016" t="n">
+        <v>3626</v>
+      </c>
+      <c r="G1016" t="n">
+        <v>727</v>
+      </c>
+      <c r="H1016" t="n">
+        <v>175</v>
+      </c>
+      <c r="I1016" t="n">
+        <v>320</v>
+      </c>
+      <c r="J1016" t="n">
+        <v>78</v>
+      </c>
+      <c r="K1016" t="n">
+        <v>87</v>
+      </c>
+      <c r="L1016" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1016" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:11:54</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>10:11:54</t>
+        </is>
+      </c>
+      <c r="D1017" t="n">
+        <v>5762</v>
+      </c>
+      <c r="E1017" t="n">
+        <v>1401</v>
+      </c>
+      <c r="F1017" t="n">
+        <v>3639</v>
+      </c>
+      <c r="G1017" t="n">
+        <v>722</v>
+      </c>
+      <c r="H1017" t="n">
+        <v>173</v>
+      </c>
+      <c r="I1017" t="n">
+        <v>319</v>
+      </c>
+      <c r="J1017" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1017" t="n">
+        <v>87</v>
+      </c>
+      <c r="L1017" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1017" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:12:13</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>10:12:13</t>
+        </is>
+      </c>
+      <c r="D1018" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1018" t="n">
+        <v>1423</v>
+      </c>
+      <c r="F1018" t="n">
+        <v>3608</v>
+      </c>
+      <c r="G1018" t="n">
+        <v>732</v>
+      </c>
+      <c r="H1018" t="n">
+        <v>174</v>
+      </c>
+      <c r="I1018" t="n">
+        <v>314</v>
+      </c>
+      <c r="J1018" t="n">
+        <v>80</v>
+      </c>
+      <c r="K1018" t="n">
+        <v>86</v>
+      </c>
+      <c r="L1018" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1018" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:12:23</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>10:12:23</t>
+        </is>
+      </c>
+      <c r="D1019" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1019" t="n">
+        <v>1426</v>
+      </c>
+      <c r="F1019" t="n">
+        <v>3602</v>
+      </c>
+      <c r="G1019" t="n">
+        <v>738</v>
+      </c>
+      <c r="H1019" t="n">
+        <v>177</v>
+      </c>
+      <c r="I1019" t="n">
+        <v>314</v>
+      </c>
+      <c r="J1019" t="n">
+        <v>82</v>
+      </c>
+      <c r="K1019" t="n">
+        <v>88</v>
+      </c>
+      <c r="L1019" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1019" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:12:33</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>10:12:33</t>
+        </is>
+      </c>
+      <c r="D1020" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1020" t="n">
+        <v>1420</v>
+      </c>
+      <c r="F1020" t="n">
+        <v>3613</v>
+      </c>
+      <c r="G1020" t="n">
+        <v>732</v>
+      </c>
+      <c r="H1020" t="n">
+        <v>178</v>
+      </c>
+      <c r="I1020" t="n">
+        <v>310</v>
+      </c>
+      <c r="J1020" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1020" t="n">
+        <v>87</v>
+      </c>
+      <c r="L1020" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1020" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:12:45</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>10:12:45</t>
+        </is>
+      </c>
+      <c r="D1021" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1021" t="n">
+        <v>1414</v>
+      </c>
+      <c r="F1021" t="n">
+        <v>3615</v>
+      </c>
+      <c r="G1021" t="n">
+        <v>737</v>
+      </c>
+      <c r="H1021" t="n">
+        <v>174</v>
+      </c>
+      <c r="I1021" t="n">
+        <v>321</v>
+      </c>
+      <c r="J1021" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1021" t="n">
+        <v>86</v>
+      </c>
+      <c r="L1021" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1021" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:12:54</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>10:12:54</t>
+        </is>
+      </c>
+      <c r="D1022" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1022" t="n">
+        <v>1414</v>
+      </c>
+      <c r="F1022" t="n">
+        <v>3626</v>
+      </c>
+      <c r="G1022" t="n">
+        <v>724</v>
+      </c>
+      <c r="H1022" t="n">
+        <v>173</v>
+      </c>
+      <c r="I1022" t="n">
+        <v>321</v>
+      </c>
+      <c r="J1022" t="n">
+        <v>75</v>
+      </c>
+      <c r="K1022" t="n">
+        <v>90</v>
+      </c>
+      <c r="L1022" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1022" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:13:06</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>10:13:06</t>
+        </is>
+      </c>
+      <c r="D1023" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1023" t="n">
+        <v>1412</v>
+      </c>
+      <c r="F1023" t="n">
+        <v>3624</v>
+      </c>
+      <c r="G1023" t="n">
+        <v>730</v>
+      </c>
+      <c r="H1023" t="n">
+        <v>173</v>
+      </c>
+      <c r="I1023" t="n">
+        <v>327</v>
+      </c>
+      <c r="J1023" t="n">
+        <v>74</v>
+      </c>
+      <c r="K1023" t="n">
+        <v>89</v>
+      </c>
+      <c r="L1023" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1023" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:13:17</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>10:13:17</t>
+        </is>
+      </c>
+      <c r="D1024" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1024" t="n">
+        <v>1388</v>
+      </c>
+      <c r="F1024" t="n">
+        <v>3643</v>
+      </c>
+      <c r="G1024" t="n">
+        <v>734</v>
+      </c>
+      <c r="H1024" t="n">
+        <v>177</v>
+      </c>
+      <c r="I1024" t="n">
+        <v>329</v>
+      </c>
+      <c r="J1024" t="n">
+        <v>76</v>
+      </c>
+      <c r="K1024" t="n">
+        <v>91</v>
+      </c>
+      <c r="L1024" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1024" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:13:28</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>10:13:28</t>
+        </is>
+      </c>
+      <c r="D1025" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1025" t="n">
+        <v>1420</v>
+      </c>
+      <c r="F1025" t="n">
+        <v>3622</v>
+      </c>
+      <c r="G1025" t="n">
+        <v>723</v>
+      </c>
+      <c r="H1025" t="n">
+        <v>178</v>
+      </c>
+      <c r="I1025" t="n">
+        <v>331</v>
+      </c>
+      <c r="J1025" t="n">
+        <v>78</v>
+      </c>
+      <c r="K1025" t="n">
+        <v>90</v>
+      </c>
+      <c r="L1025" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1025" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:13:37</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>10:13:37</t>
+        </is>
+      </c>
+      <c r="D1026" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1026" t="n">
+        <v>1421</v>
+      </c>
+      <c r="F1026" t="n">
+        <v>3613</v>
+      </c>
+      <c r="G1026" t="n">
+        <v>730</v>
+      </c>
+      <c r="H1026" t="n">
+        <v>183</v>
+      </c>
+      <c r="I1026" t="n">
+        <v>322</v>
+      </c>
+      <c r="J1026" t="n">
+        <v>78</v>
+      </c>
+      <c r="K1026" t="n">
+        <v>90</v>
+      </c>
+      <c r="L1026" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1026" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:13:47</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>10:13:47</t>
+        </is>
+      </c>
+      <c r="D1027" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1027" t="n">
+        <v>1425</v>
+      </c>
+      <c r="F1027" t="n">
+        <v>3601</v>
+      </c>
+      <c r="G1027" t="n">
+        <v>739</v>
+      </c>
+      <c r="H1027" t="n">
+        <v>184</v>
+      </c>
+      <c r="I1027" t="n">
+        <v>316</v>
+      </c>
+      <c r="J1027" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1027" t="n">
+        <v>89</v>
+      </c>
+      <c r="L1027" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1027" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:13:57</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>10:13:57</t>
+        </is>
+      </c>
+      <c r="D1028" t="n">
+        <v>5767</v>
+      </c>
+      <c r="E1028" t="n">
+        <v>1427</v>
+      </c>
+      <c r="F1028" t="n">
+        <v>3604</v>
+      </c>
+      <c r="G1028" t="n">
+        <v>736</v>
+      </c>
+      <c r="H1028" t="n">
+        <v>188</v>
+      </c>
+      <c r="I1028" t="n">
+        <v>324</v>
+      </c>
+      <c r="J1028" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1028" t="n">
+        <v>88</v>
+      </c>
+      <c r="L1028" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1028" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:14:07</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>10:14:07</t>
+        </is>
+      </c>
+      <c r="D1029" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1029" t="n">
+        <v>1433</v>
+      </c>
+      <c r="F1029" t="n">
+        <v>3610</v>
+      </c>
+      <c r="G1029" t="n">
+        <v>722</v>
+      </c>
+      <c r="H1029" t="n">
+        <v>187</v>
+      </c>
+      <c r="I1029" t="n">
+        <v>334</v>
+      </c>
+      <c r="J1029" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1029" t="n">
+        <v>87</v>
+      </c>
+      <c r="L1029" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1029" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:14:18</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>10:14:18</t>
+        </is>
+      </c>
+      <c r="D1030" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1030" t="n">
+        <v>1414</v>
+      </c>
+      <c r="F1030" t="n">
+        <v>3619</v>
+      </c>
+      <c r="G1030" t="n">
+        <v>730</v>
+      </c>
+      <c r="H1030" t="n">
+        <v>184</v>
+      </c>
+      <c r="I1030" t="n">
+        <v>329</v>
+      </c>
+      <c r="J1030" t="n">
+        <v>83</v>
+      </c>
+      <c r="K1030" t="n">
+        <v>90</v>
+      </c>
+      <c r="L1030" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1030" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:14:27</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>10:14:27</t>
+        </is>
+      </c>
+      <c r="D1031" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1031" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F1031" t="n">
+        <v>3631</v>
+      </c>
+      <c r="G1031" t="n">
+        <v>733</v>
+      </c>
+      <c r="H1031" t="n">
+        <v>180</v>
+      </c>
+      <c r="I1031" t="n">
+        <v>345</v>
+      </c>
+      <c r="J1031" t="n">
+        <v>82</v>
+      </c>
+      <c r="K1031" t="n">
+        <v>90</v>
+      </c>
+      <c r="L1031" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1031" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:14:37</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>10:14:37</t>
+        </is>
+      </c>
+      <c r="D1032" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1032" t="n">
+        <v>1364</v>
+      </c>
+      <c r="F1032" t="n">
+        <v>3667</v>
+      </c>
+      <c r="G1032" t="n">
+        <v>733</v>
+      </c>
+      <c r="H1032" t="n">
+        <v>176</v>
+      </c>
+      <c r="I1032" t="n">
+        <v>344</v>
+      </c>
+      <c r="J1032" t="n">
+        <v>80</v>
+      </c>
+      <c r="K1032" t="n">
+        <v>90</v>
+      </c>
+      <c r="L1032" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1032" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:14:47</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>10:14:47</t>
+        </is>
+      </c>
+      <c r="D1033" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1033" t="n">
+        <v>1350</v>
+      </c>
+      <c r="F1033" t="n">
+        <v>3685</v>
+      </c>
+      <c r="G1033" t="n">
+        <v>730</v>
+      </c>
+      <c r="H1033" t="n">
+        <v>181</v>
+      </c>
+      <c r="I1033" t="n">
+        <v>348</v>
+      </c>
+      <c r="J1033" t="n">
+        <v>80</v>
+      </c>
+      <c r="K1033" t="n">
+        <v>94</v>
+      </c>
+      <c r="L1033" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1033" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:14:57</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>10:14:57</t>
+        </is>
+      </c>
+      <c r="D1034" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1034" t="n">
+        <v>1351</v>
+      </c>
+      <c r="F1034" t="n">
+        <v>3683</v>
+      </c>
+      <c r="G1034" t="n">
+        <v>732</v>
+      </c>
+      <c r="H1034" t="n">
+        <v>183</v>
+      </c>
+      <c r="I1034" t="n">
+        <v>352</v>
+      </c>
+      <c r="J1034" t="n">
+        <v>81</v>
+      </c>
+      <c r="K1034" t="n">
+        <v>97</v>
+      </c>
+      <c r="L1034" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1034" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:15:07</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>10:15:07</t>
+        </is>
+      </c>
+      <c r="D1035" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1035" t="n">
+        <v>1346</v>
+      </c>
+      <c r="F1035" t="n">
+        <v>3695</v>
+      </c>
+      <c r="G1035" t="n">
+        <v>724</v>
+      </c>
+      <c r="H1035" t="n">
+        <v>185</v>
+      </c>
+      <c r="I1035" t="n">
+        <v>358</v>
+      </c>
+      <c r="J1035" t="n">
+        <v>81</v>
+      </c>
+      <c r="K1035" t="n">
+        <v>93</v>
+      </c>
+      <c r="L1035" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1035" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:15:17</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>10:15:17</t>
+        </is>
+      </c>
+      <c r="D1036" t="n">
+        <v>5762</v>
+      </c>
+      <c r="E1036" t="n">
+        <v>1292</v>
+      </c>
+      <c r="F1036" t="n">
+        <v>3747</v>
+      </c>
+      <c r="G1036" t="n">
+        <v>723</v>
+      </c>
+      <c r="H1036" t="n">
+        <v>181</v>
+      </c>
+      <c r="I1036" t="n">
+        <v>370</v>
+      </c>
+      <c r="J1036" t="n">
+        <v>82</v>
+      </c>
+      <c r="K1036" t="n">
+        <v>94</v>
+      </c>
+      <c r="L1036" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1036" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:15:27</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>10:15:27</t>
+        </is>
+      </c>
+      <c r="D1037" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1037" t="n">
+        <v>1256</v>
+      </c>
+      <c r="F1037" t="n">
+        <v>3780</v>
+      </c>
+      <c r="G1037" t="n">
+        <v>729</v>
+      </c>
+      <c r="H1037" t="n">
+        <v>177</v>
+      </c>
+      <c r="I1037" t="n">
+        <v>370</v>
+      </c>
+      <c r="J1037" t="n">
+        <v>81</v>
+      </c>
+      <c r="K1037" t="n">
+        <v>96</v>
+      </c>
+      <c r="L1037" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1037" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:15:37</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>10:15:37</t>
+        </is>
+      </c>
+      <c r="D1038" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1038" t="n">
+        <v>1262</v>
+      </c>
+      <c r="F1038" t="n">
+        <v>3793</v>
+      </c>
+      <c r="G1038" t="n">
+        <v>710</v>
+      </c>
+      <c r="H1038" t="n">
+        <v>178</v>
+      </c>
+      <c r="I1038" t="n">
+        <v>361</v>
+      </c>
+      <c r="J1038" t="n">
+        <v>80</v>
+      </c>
+      <c r="K1038" t="n">
+        <v>95</v>
+      </c>
+      <c r="L1038" t="n">
+        <v>33</v>
+      </c>
+      <c r="M1038" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:15:47</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>10:15:47</t>
+        </is>
+      </c>
+      <c r="D1039" t="n">
+        <v>5762</v>
+      </c>
+      <c r="E1039" t="n">
+        <v>1266</v>
+      </c>
+      <c r="F1039" t="n">
+        <v>3775</v>
+      </c>
+      <c r="G1039" t="n">
+        <v>721</v>
+      </c>
+      <c r="H1039" t="n">
+        <v>177</v>
+      </c>
+      <c r="I1039" t="n">
+        <v>364</v>
+      </c>
+      <c r="J1039" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1039" t="n">
+        <v>93</v>
+      </c>
+      <c r="L1039" t="n">
+        <v>33</v>
+      </c>
+      <c r="M1039" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:15:57</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>10:15:57</t>
+        </is>
+      </c>
+      <c r="D1040" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1040" t="n">
+        <v>1270</v>
+      </c>
+      <c r="F1040" t="n">
+        <v>3765</v>
+      </c>
+      <c r="G1040" t="n">
+        <v>731</v>
+      </c>
+      <c r="H1040" t="n">
+        <v>178</v>
+      </c>
+      <c r="I1040" t="n">
+        <v>363</v>
+      </c>
+      <c r="J1040" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1040" t="n">
+        <v>94</v>
+      </c>
+      <c r="L1040" t="n">
+        <v>32</v>
+      </c>
+      <c r="M1040" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:16:07</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>10:16:07</t>
+        </is>
+      </c>
+      <c r="D1041" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1041" t="n">
+        <v>1290</v>
+      </c>
+      <c r="F1041" t="n">
+        <v>3751</v>
+      </c>
+      <c r="G1041" t="n">
+        <v>723</v>
+      </c>
+      <c r="H1041" t="n">
+        <v>178</v>
+      </c>
+      <c r="I1041" t="n">
+        <v>361</v>
+      </c>
+      <c r="J1041" t="n">
+        <v>80</v>
+      </c>
+      <c r="K1041" t="n">
+        <v>92</v>
+      </c>
+      <c r="L1041" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1041" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:16:17</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>10:16:17</t>
+        </is>
+      </c>
+      <c r="D1042" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1042" t="n">
+        <v>1288</v>
+      </c>
+      <c r="F1042" t="n">
+        <v>3758</v>
+      </c>
+      <c r="G1042" t="n">
+        <v>718</v>
+      </c>
+      <c r="H1042" t="n">
+        <v>177</v>
+      </c>
+      <c r="I1042" t="n">
+        <v>373</v>
+      </c>
+      <c r="J1042" t="n">
+        <v>80</v>
+      </c>
+      <c r="K1042" t="n">
+        <v>92</v>
+      </c>
+      <c r="L1042" t="n">
+        <v>30</v>
+      </c>
+      <c r="M1042" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:16:27</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>10:16:27</t>
+        </is>
+      </c>
+      <c r="D1043" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1043" t="n">
+        <v>1291</v>
+      </c>
+      <c r="F1043" t="n">
+        <v>3754</v>
+      </c>
+      <c r="G1043" t="n">
+        <v>719</v>
+      </c>
+      <c r="H1043" t="n">
+        <v>178</v>
+      </c>
+      <c r="I1043" t="n">
+        <v>362</v>
+      </c>
+      <c r="J1043" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1043" t="n">
+        <v>92</v>
+      </c>
+      <c r="L1043" t="n">
+        <v>30</v>
+      </c>
+      <c r="M1043" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:16:37</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>10:16:37</t>
+        </is>
+      </c>
+      <c r="D1044" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1044" t="n">
+        <v>1248</v>
+      </c>
+      <c r="F1044" t="n">
+        <v>3787</v>
+      </c>
+      <c r="G1044" t="n">
+        <v>730</v>
+      </c>
+      <c r="H1044" t="n">
+        <v>176</v>
+      </c>
+      <c r="I1044" t="n">
+        <v>364</v>
+      </c>
+      <c r="J1044" t="n">
+        <v>78</v>
+      </c>
+      <c r="K1044" t="n">
+        <v>95</v>
+      </c>
+      <c r="L1044" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1044" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:16:48</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>10:16:48</t>
+        </is>
+      </c>
+      <c r="D1045" t="n">
+        <v>5767</v>
+      </c>
+      <c r="E1045" t="n">
+        <v>1278</v>
+      </c>
+      <c r="F1045" t="n">
+        <v>3759</v>
+      </c>
+      <c r="G1045" t="n">
+        <v>730</v>
+      </c>
+      <c r="H1045" t="n">
+        <v>178</v>
+      </c>
+      <c r="I1045" t="n">
+        <v>357</v>
+      </c>
+      <c r="J1045" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1045" t="n">
+        <v>95</v>
+      </c>
+      <c r="L1045" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1045" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:16:58</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>10:16:58</t>
+        </is>
+      </c>
+      <c r="D1046" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1046" t="n">
+        <v>1311</v>
+      </c>
+      <c r="F1046" t="n">
+        <v>3726</v>
+      </c>
+      <c r="G1046" t="n">
+        <v>727</v>
+      </c>
+      <c r="H1046" t="n">
+        <v>177</v>
+      </c>
+      <c r="I1046" t="n">
+        <v>358</v>
+      </c>
+      <c r="J1046" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1046" t="n">
+        <v>93</v>
+      </c>
+      <c r="L1046" t="n">
+        <v>30</v>
+      </c>
+      <c r="M1046" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:17:09</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>10:17:09</t>
+        </is>
+      </c>
+      <c r="D1047" t="n">
+        <v>5761</v>
+      </c>
+      <c r="E1047" t="n">
+        <v>1317</v>
+      </c>
+      <c r="F1047" t="n">
+        <v>3729</v>
+      </c>
+      <c r="G1047" t="n">
+        <v>715</v>
+      </c>
+      <c r="H1047" t="n">
+        <v>173</v>
+      </c>
+      <c r="I1047" t="n">
+        <v>354</v>
+      </c>
+      <c r="J1047" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1047" t="n">
+        <v>93</v>
+      </c>
+      <c r="L1047" t="n">
+        <v>30</v>
+      </c>
+      <c r="M1047" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:17:19</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>10:17:19</t>
+        </is>
+      </c>
+      <c r="D1048" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1048" t="n">
+        <v>1319</v>
+      </c>
+      <c r="F1048" t="n">
+        <v>3715</v>
+      </c>
+      <c r="G1048" t="n">
+        <v>730</v>
+      </c>
+      <c r="H1048" t="n">
+        <v>173</v>
+      </c>
+      <c r="I1048" t="n">
+        <v>350</v>
+      </c>
+      <c r="J1048" t="n">
+        <v>80</v>
+      </c>
+      <c r="K1048" t="n">
+        <v>92</v>
+      </c>
+      <c r="L1048" t="n">
+        <v>30</v>
+      </c>
+      <c r="M1048" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:18:51</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>10:18:51</t>
+        </is>
+      </c>
+      <c r="D1049" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1049" t="n">
+        <v>1332</v>
+      </c>
+      <c r="F1049" t="n">
+        <v>3709</v>
+      </c>
+      <c r="G1049" t="n">
+        <v>725</v>
+      </c>
+      <c r="H1049" t="n">
+        <v>182</v>
+      </c>
+      <c r="I1049" t="n">
+        <v>341</v>
+      </c>
+      <c r="J1049" t="n">
+        <v>80</v>
+      </c>
+      <c r="K1049" t="n">
+        <v>94</v>
+      </c>
+      <c r="L1049" t="n">
+        <v>30</v>
+      </c>
+      <c r="M1049" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:19:02</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>10:19:02</t>
+        </is>
+      </c>
+      <c r="D1050" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1050" t="n">
+        <v>1330</v>
+      </c>
+      <c r="F1050" t="n">
+        <v>3707</v>
+      </c>
+      <c r="G1050" t="n">
+        <v>726</v>
+      </c>
+      <c r="H1050" t="n">
+        <v>182</v>
+      </c>
+      <c r="I1050" t="n">
+        <v>340</v>
+      </c>
+      <c r="J1050" t="n">
+        <v>82</v>
+      </c>
+      <c r="K1050" t="n">
+        <v>95</v>
+      </c>
+      <c r="L1050" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1050" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:19:12</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>10:19:12</t>
+        </is>
+      </c>
+      <c r="D1051" t="n">
+        <v>5761</v>
+      </c>
+      <c r="E1051" t="n">
+        <v>1316</v>
+      </c>
+      <c r="F1051" t="n">
+        <v>3718</v>
+      </c>
+      <c r="G1051" t="n">
+        <v>727</v>
+      </c>
+      <c r="H1051" t="n">
+        <v>181</v>
+      </c>
+      <c r="I1051" t="n">
+        <v>351</v>
+      </c>
+      <c r="J1051" t="n">
+        <v>81</v>
+      </c>
+      <c r="K1051" t="n">
+        <v>95</v>
+      </c>
+      <c r="L1051" t="n">
+        <v>32</v>
+      </c>
+      <c r="M1051" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:19:23</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>10:19:23</t>
+        </is>
+      </c>
+      <c r="D1052" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1052" t="n">
+        <v>1309</v>
+      </c>
+      <c r="F1052" t="n">
+        <v>3738</v>
+      </c>
+      <c r="G1052" t="n">
+        <v>718</v>
+      </c>
+      <c r="H1052" t="n">
+        <v>176</v>
+      </c>
+      <c r="I1052" t="n">
+        <v>354</v>
+      </c>
+      <c r="J1052" t="n">
+        <v>81</v>
+      </c>
+      <c r="K1052" t="n">
+        <v>93</v>
+      </c>
+      <c r="L1052" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1052" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:19:33</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>10:19:33</t>
+        </is>
+      </c>
+      <c r="D1053" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1053" t="n">
+        <v>1333</v>
+      </c>
+      <c r="F1053" t="n">
+        <v>3727</v>
+      </c>
+      <c r="G1053" t="n">
+        <v>704</v>
+      </c>
+      <c r="H1053" t="n">
+        <v>181</v>
+      </c>
+      <c r="I1053" t="n">
+        <v>351</v>
+      </c>
+      <c r="J1053" t="n">
+        <v>81</v>
+      </c>
+      <c r="K1053" t="n">
+        <v>94</v>
+      </c>
+      <c r="L1053" t="n">
+        <v>30</v>
+      </c>
+      <c r="M1053" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:19:45</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>10:19:45</t>
+        </is>
+      </c>
+      <c r="D1054" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1054" t="n">
+        <v>1335</v>
+      </c>
+      <c r="F1054" t="n">
+        <v>3712</v>
+      </c>
+      <c r="G1054" t="n">
+        <v>718</v>
+      </c>
+      <c r="H1054" t="n">
+        <v>180</v>
+      </c>
+      <c r="I1054" t="n">
+        <v>337</v>
+      </c>
+      <c r="J1054" t="n">
+        <v>83</v>
+      </c>
+      <c r="K1054" t="n">
+        <v>92</v>
+      </c>
+      <c r="L1054" t="n">
+        <v>30</v>
+      </c>
+      <c r="M1054" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:19:56</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>10:19:56</t>
+        </is>
+      </c>
+      <c r="D1055" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1055" t="n">
+        <v>1335</v>
+      </c>
+      <c r="F1055" t="n">
+        <v>3700</v>
+      </c>
+      <c r="G1055" t="n">
+        <v>728</v>
+      </c>
+      <c r="H1055" t="n">
+        <v>181</v>
+      </c>
+      <c r="I1055" t="n">
+        <v>344</v>
+      </c>
+      <c r="J1055" t="n">
+        <v>83</v>
+      </c>
+      <c r="K1055" t="n">
+        <v>92</v>
+      </c>
+      <c r="L1055" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1055" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:20:07</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>10:20:07</t>
+        </is>
+      </c>
+      <c r="D1056" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1056" t="n">
+        <v>1346</v>
+      </c>
+      <c r="F1056" t="n">
+        <v>3705</v>
+      </c>
+      <c r="G1056" t="n">
+        <v>714</v>
+      </c>
+      <c r="H1056" t="n">
+        <v>188</v>
+      </c>
+      <c r="I1056" t="n">
+        <v>341</v>
+      </c>
+      <c r="J1056" t="n">
+        <v>82</v>
+      </c>
+      <c r="K1056" t="n">
+        <v>93</v>
+      </c>
+      <c r="L1056" t="n">
+        <v>32</v>
+      </c>
+      <c r="M1056" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:20:17</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>10:20:17</t>
+        </is>
+      </c>
+      <c r="D1057" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1057" t="n">
+        <v>1334</v>
+      </c>
+      <c r="F1057" t="n">
+        <v>3714</v>
+      </c>
+      <c r="G1057" t="n">
+        <v>718</v>
+      </c>
+      <c r="H1057" t="n">
+        <v>188</v>
+      </c>
+      <c r="I1057" t="n">
+        <v>345</v>
+      </c>
+      <c r="J1057" t="n">
+        <v>82</v>
+      </c>
+      <c r="K1057" t="n">
+        <v>90</v>
+      </c>
+      <c r="L1057" t="n">
+        <v>32</v>
+      </c>
+      <c r="M1057" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:20:27</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>10:20:27</t>
+        </is>
+      </c>
+      <c r="D1058" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1058" t="n">
+        <v>1340</v>
+      </c>
+      <c r="F1058" t="n">
+        <v>3712</v>
+      </c>
+      <c r="G1058" t="n">
+        <v>712</v>
+      </c>
+      <c r="H1058" t="n">
+        <v>190</v>
+      </c>
+      <c r="I1058" t="n">
+        <v>343</v>
+      </c>
+      <c r="J1058" t="n">
+        <v>80</v>
+      </c>
+      <c r="K1058" t="n">
+        <v>91</v>
+      </c>
+      <c r="L1058" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1058" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:20:37</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>10:20:37</t>
+        </is>
+      </c>
+      <c r="D1059" t="n">
+        <v>5761</v>
+      </c>
+      <c r="E1059" t="n">
+        <v>1335</v>
+      </c>
+      <c r="F1059" t="n">
+        <v>3713</v>
+      </c>
+      <c r="G1059" t="n">
+        <v>713</v>
+      </c>
+      <c r="H1059" t="n">
+        <v>186</v>
+      </c>
+      <c r="I1059" t="n">
+        <v>341</v>
+      </c>
+      <c r="J1059" t="n">
+        <v>78</v>
+      </c>
+      <c r="K1059" t="n">
+        <v>92</v>
+      </c>
+      <c r="L1059" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1059" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:20:48</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>10:20:48</t>
+        </is>
+      </c>
+      <c r="D1060" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1060" t="n">
+        <v>1335</v>
+      </c>
+      <c r="F1060" t="n">
+        <v>3715</v>
+      </c>
+      <c r="G1060" t="n">
+        <v>714</v>
+      </c>
+      <c r="H1060" t="n">
+        <v>185</v>
+      </c>
+      <c r="I1060" t="n">
+        <v>348</v>
+      </c>
+      <c r="J1060" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1060" t="n">
+        <v>91</v>
+      </c>
+      <c r="L1060" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1060" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:20:58</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>10:20:58</t>
+        </is>
+      </c>
+      <c r="D1061" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1061" t="n">
+        <v>1330</v>
+      </c>
+      <c r="F1061" t="n">
+        <v>3728</v>
+      </c>
+      <c r="G1061" t="n">
+        <v>705</v>
+      </c>
+      <c r="H1061" t="n">
+        <v>182</v>
+      </c>
+      <c r="I1061" t="n">
+        <v>353</v>
+      </c>
+      <c r="J1061" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1061" t="n">
+        <v>93</v>
+      </c>
+      <c r="L1061" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1061" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:21:09</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>10:21:09</t>
+        </is>
+      </c>
+      <c r="D1062" t="n">
+        <v>5761</v>
+      </c>
+      <c r="E1062" t="n">
+        <v>1319</v>
+      </c>
+      <c r="F1062" t="n">
+        <v>3734</v>
+      </c>
+      <c r="G1062" t="n">
+        <v>708</v>
+      </c>
+      <c r="H1062" t="n">
+        <v>180</v>
+      </c>
+      <c r="I1062" t="n">
+        <v>351</v>
+      </c>
+      <c r="J1062" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1062" t="n">
+        <v>93</v>
+      </c>
+      <c r="L1062" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1062" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:21:20</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>10:21:20</t>
+        </is>
+      </c>
+      <c r="D1063" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1063" t="n">
+        <v>1319</v>
+      </c>
+      <c r="F1063" t="n">
+        <v>3736</v>
+      </c>
+      <c r="G1063" t="n">
+        <v>709</v>
+      </c>
+      <c r="H1063" t="n">
+        <v>182</v>
+      </c>
+      <c r="I1063" t="n">
+        <v>350</v>
+      </c>
+      <c r="J1063" t="n">
+        <v>76</v>
+      </c>
+      <c r="K1063" t="n">
+        <v>91</v>
+      </c>
+      <c r="L1063" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1063" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:21:31</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>10:21:31</t>
+        </is>
+      </c>
+      <c r="D1064" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1064" t="n">
+        <v>1317</v>
+      </c>
+      <c r="F1064" t="n">
+        <v>3730</v>
+      </c>
+      <c r="G1064" t="n">
+        <v>717</v>
+      </c>
+      <c r="H1064" t="n">
+        <v>180</v>
+      </c>
+      <c r="I1064" t="n">
+        <v>338</v>
+      </c>
+      <c r="J1064" t="n">
+        <v>76</v>
+      </c>
+      <c r="K1064" t="n">
+        <v>91</v>
+      </c>
+      <c r="L1064" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1064" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:21:42</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>10:21:42</t>
+        </is>
+      </c>
+      <c r="D1065" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1065" t="n">
+        <v>1329</v>
+      </c>
+      <c r="F1065" t="n">
+        <v>3714</v>
+      </c>
+      <c r="G1065" t="n">
+        <v>721</v>
+      </c>
+      <c r="H1065" t="n">
+        <v>187</v>
+      </c>
+      <c r="I1065" t="n">
+        <v>344</v>
+      </c>
+      <c r="J1065" t="n">
+        <v>76</v>
+      </c>
+      <c r="K1065" t="n">
+        <v>95</v>
+      </c>
+      <c r="L1065" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1065" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:21:51</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>10:21:51</t>
+        </is>
+      </c>
+      <c r="D1066" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1066" t="n">
+        <v>1349</v>
+      </c>
+      <c r="F1066" t="n">
+        <v>3681</v>
+      </c>
+      <c r="G1066" t="n">
+        <v>733</v>
+      </c>
+      <c r="H1066" t="n">
+        <v>190</v>
+      </c>
+      <c r="I1066" t="n">
+        <v>343</v>
+      </c>
+      <c r="J1066" t="n">
+        <v>77</v>
+      </c>
+      <c r="K1066" t="n">
+        <v>92</v>
+      </c>
+      <c r="L1066" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1066" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:22:02</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>10:22:02</t>
+        </is>
+      </c>
+      <c r="D1067" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1067" t="n">
+        <v>1364</v>
+      </c>
+      <c r="F1067" t="n">
+        <v>3679</v>
+      </c>
+      <c r="G1067" t="n">
+        <v>722</v>
+      </c>
+      <c r="H1067" t="n">
+        <v>191</v>
+      </c>
+      <c r="I1067" t="n">
+        <v>334</v>
+      </c>
+      <c r="J1067" t="n">
+        <v>76</v>
+      </c>
+      <c r="K1067" t="n">
+        <v>93</v>
+      </c>
+      <c r="L1067" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1067" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:22:12</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>10:22:12</t>
+        </is>
+      </c>
+      <c r="D1068" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1068" t="n">
+        <v>1363</v>
+      </c>
+      <c r="F1068" t="n">
+        <v>3680</v>
+      </c>
+      <c r="G1068" t="n">
+        <v>720</v>
+      </c>
+      <c r="H1068" t="n">
+        <v>193</v>
+      </c>
+      <c r="I1068" t="n">
+        <v>338</v>
+      </c>
+      <c r="J1068" t="n">
+        <v>77</v>
+      </c>
+      <c r="K1068" t="n">
+        <v>92</v>
+      </c>
+      <c r="L1068" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1068" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:22:23</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>10:22:23</t>
+        </is>
+      </c>
+      <c r="D1069" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1069" t="n">
+        <v>1364</v>
+      </c>
+      <c r="F1069" t="n">
+        <v>3680</v>
+      </c>
+      <c r="G1069" t="n">
+        <v>719</v>
+      </c>
+      <c r="H1069" t="n">
+        <v>190</v>
+      </c>
+      <c r="I1069" t="n">
+        <v>336</v>
+      </c>
+      <c r="J1069" t="n">
+        <v>77</v>
+      </c>
+      <c r="K1069" t="n">
+        <v>90</v>
+      </c>
+      <c r="L1069" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1069" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:22:32</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>10:22:32</t>
+        </is>
+      </c>
+      <c r="D1070" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1070" t="n">
+        <v>1397</v>
+      </c>
+      <c r="F1070" t="n">
+        <v>3645</v>
+      </c>
+      <c r="G1070" t="n">
+        <v>721</v>
+      </c>
+      <c r="H1070" t="n">
+        <v>192</v>
+      </c>
+      <c r="I1070" t="n">
+        <v>325</v>
+      </c>
+      <c r="J1070" t="n">
+        <v>78</v>
+      </c>
+      <c r="K1070" t="n">
+        <v>89</v>
+      </c>
+      <c r="L1070" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1070" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:22:42</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>10:22:42</t>
+        </is>
+      </c>
+      <c r="D1071" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1071" t="n">
+        <v>1416</v>
+      </c>
+      <c r="F1071" t="n">
+        <v>3627</v>
+      </c>
+      <c r="G1071" t="n">
+        <v>720</v>
+      </c>
+      <c r="H1071" t="n">
+        <v>192</v>
+      </c>
+      <c r="I1071" t="n">
+        <v>325</v>
+      </c>
+      <c r="J1071" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1071" t="n">
+        <v>90</v>
+      </c>
+      <c r="L1071" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1071" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:22:53</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>10:22:53</t>
+        </is>
+      </c>
+      <c r="D1072" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1072" t="n">
+        <v>1413</v>
+      </c>
+      <c r="F1072" t="n">
+        <v>3624</v>
+      </c>
+      <c r="G1072" t="n">
+        <v>729</v>
+      </c>
+      <c r="H1072" t="n">
+        <v>191</v>
+      </c>
+      <c r="I1072" t="n">
+        <v>328</v>
+      </c>
+      <c r="J1072" t="n">
+        <v>79</v>
+      </c>
+      <c r="K1072" t="n">
+        <v>90</v>
+      </c>
+      <c r="L1072" t="n">
+        <v>31</v>
+      </c>
+      <c r="M1072" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:37:32</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>10:37:32</t>
+        </is>
+      </c>
+      <c r="D1073" t="n">
+        <v>4031</v>
+      </c>
+      <c r="E1073" t="n">
+        <v>918</v>
+      </c>
+      <c r="F1073" t="n">
+        <v>2571</v>
+      </c>
+      <c r="G1073" t="n">
+        <v>542</v>
+      </c>
+      <c r="H1073" t="n">
+        <v>130</v>
+      </c>
+      <c r="I1073" t="n">
+        <v>248</v>
+      </c>
+      <c r="J1073" t="n">
+        <v>50</v>
+      </c>
+      <c r="K1073" t="n">
+        <v>62</v>
+      </c>
+      <c r="L1073" t="n">
+        <v>22</v>
+      </c>
+      <c r="M1073" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:37:44</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>10:37:44</t>
+        </is>
+      </c>
+      <c r="D1074" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1074" t="n">
+        <v>1326</v>
+      </c>
+      <c r="F1074" t="n">
+        <v>3721</v>
+      </c>
+      <c r="G1074" t="n">
+        <v>719</v>
+      </c>
+      <c r="H1074" t="n">
+        <v>190</v>
+      </c>
+      <c r="I1074" t="n">
+        <v>375</v>
+      </c>
+      <c r="J1074" t="n">
+        <v>86</v>
+      </c>
+      <c r="K1074" t="n">
+        <v>91</v>
+      </c>
+      <c r="L1074" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1074" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:56:33</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>10:56:33</t>
+        </is>
+      </c>
+      <c r="D1075" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1075" t="n">
+        <v>1207</v>
+      </c>
+      <c r="F1075" t="n">
+        <v>3859</v>
+      </c>
+      <c r="G1075" t="n">
+        <v>697</v>
+      </c>
+      <c r="H1075" t="n">
+        <v>182</v>
+      </c>
+      <c r="I1075" t="n">
+        <v>419</v>
+      </c>
+      <c r="J1075" t="n">
+        <v>83</v>
+      </c>
+      <c r="K1075" t="n">
+        <v>107</v>
+      </c>
+      <c r="L1075" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1075" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:56:54</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>10:56:54</t>
+        </is>
+      </c>
+      <c r="D1076" t="n">
+        <v>5264</v>
+      </c>
+      <c r="E1076" t="n">
+        <v>1114</v>
+      </c>
+      <c r="F1076" t="n">
+        <v>3504</v>
+      </c>
+      <c r="G1076" t="n">
+        <v>646</v>
+      </c>
+      <c r="H1076" t="n">
+        <v>164</v>
+      </c>
+      <c r="I1076" t="n">
+        <v>379</v>
+      </c>
+      <c r="J1076" t="n">
+        <v>73</v>
+      </c>
+      <c r="K1076" t="n">
+        <v>93</v>
+      </c>
+      <c r="L1076" t="n">
+        <v>28</v>
+      </c>
+      <c r="M1076" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:57:04</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>10:57:04</t>
+        </is>
+      </c>
+      <c r="D1077" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1077" t="n">
+        <v>1225</v>
+      </c>
+      <c r="F1077" t="n">
+        <v>3850</v>
+      </c>
+      <c r="G1077" t="n">
+        <v>689</v>
+      </c>
+      <c r="H1077" t="n">
+        <v>186</v>
+      </c>
+      <c r="I1077" t="n">
+        <v>419</v>
+      </c>
+      <c r="J1077" t="n">
+        <v>85</v>
+      </c>
+      <c r="K1077" t="n">
+        <v>105</v>
+      </c>
+      <c r="L1077" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1077" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:57:13</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>10:57:13</t>
+        </is>
+      </c>
+      <c r="D1078" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1078" t="n">
+        <v>1229</v>
+      </c>
+      <c r="F1078" t="n">
+        <v>3838</v>
+      </c>
+      <c r="G1078" t="n">
+        <v>699</v>
+      </c>
+      <c r="H1078" t="n">
+        <v>192</v>
+      </c>
+      <c r="I1078" t="n">
+        <v>422</v>
+      </c>
+      <c r="J1078" t="n">
+        <v>86</v>
+      </c>
+      <c r="K1078" t="n">
+        <v>106</v>
+      </c>
+      <c r="L1078" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1078" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:57:24</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>10:57:24</t>
+        </is>
+      </c>
+      <c r="D1079" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1079" t="n">
+        <v>1242</v>
+      </c>
+      <c r="F1079" t="n">
+        <v>3829</v>
+      </c>
+      <c r="G1079" t="n">
+        <v>694</v>
+      </c>
+      <c r="H1079" t="n">
+        <v>191</v>
+      </c>
+      <c r="I1079" t="n">
+        <v>420</v>
+      </c>
+      <c r="J1079" t="n">
+        <v>87</v>
+      </c>
+      <c r="K1079" t="n">
+        <v>106</v>
+      </c>
+      <c r="L1079" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1079" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:57:33</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>10:57:33</t>
+        </is>
+      </c>
+      <c r="D1080" t="n">
+        <v>5762</v>
+      </c>
+      <c r="E1080" t="n">
+        <v>1219</v>
+      </c>
+      <c r="F1080" t="n">
+        <v>3843</v>
+      </c>
+      <c r="G1080" t="n">
+        <v>700</v>
+      </c>
+      <c r="H1080" t="n">
+        <v>192</v>
+      </c>
+      <c r="I1080" t="n">
+        <v>419</v>
+      </c>
+      <c r="J1080" t="n">
+        <v>86</v>
+      </c>
+      <c r="K1080" t="n">
+        <v>107</v>
+      </c>
+      <c r="L1080" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1080" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:57:43</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>10:57:43</t>
+        </is>
+      </c>
+      <c r="D1081" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1081" t="n">
+        <v>1220</v>
+      </c>
+      <c r="F1081" t="n">
+        <v>3854</v>
+      </c>
+      <c r="G1081" t="n">
+        <v>690</v>
+      </c>
+      <c r="H1081" t="n">
+        <v>188</v>
+      </c>
+      <c r="I1081" t="n">
+        <v>427</v>
+      </c>
+      <c r="J1081" t="n">
+        <v>85</v>
+      </c>
+      <c r="K1081" t="n">
+        <v>107</v>
+      </c>
+      <c r="L1081" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1081" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:57:53</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>10:57:53</t>
+        </is>
+      </c>
+      <c r="D1082" t="n">
+        <v>5764</v>
+      </c>
+      <c r="E1082" t="n">
+        <v>1229</v>
+      </c>
+      <c r="F1082" t="n">
+        <v>3846</v>
+      </c>
+      <c r="G1082" t="n">
+        <v>689</v>
+      </c>
+      <c r="H1082" t="n">
+        <v>189</v>
+      </c>
+      <c r="I1082" t="n">
+        <v>424</v>
+      </c>
+      <c r="J1082" t="n">
+        <v>86</v>
+      </c>
+      <c r="K1082" t="n">
+        <v>107</v>
+      </c>
+      <c r="L1082" t="n">
+        <v>34</v>
+      </c>
+      <c r="M1082" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>2025-12-11 10:58:04</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>10:58:04</t>
+        </is>
+      </c>
+      <c r="D1083" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1083" t="n">
+        <v>1230</v>
+      </c>
+      <c r="F1083" t="n">
+        <v>3840</v>
+      </c>
+      <c r="G1083" t="n">
+        <v>695</v>
+      </c>
+      <c r="H1083" t="n">
+        <v>192</v>
+      </c>
+      <c r="I1083" t="n">
+        <v>419</v>
+      </c>
+      <c r="J1083" t="n">
+        <v>86</v>
+      </c>
+      <c r="K1083" t="n">
+        <v>108</v>
+      </c>
+      <c r="L1083" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1083" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>2025-12-11 11:02:30</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>11:02:30</t>
+        </is>
+      </c>
+      <c r="D1084" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1084" t="n">
+        <v>1177</v>
+      </c>
+      <c r="F1084" t="n">
+        <v>3894</v>
+      </c>
+      <c r="G1084" t="n">
+        <v>695</v>
+      </c>
+      <c r="H1084" t="n">
+        <v>187</v>
+      </c>
+      <c r="I1084" t="n">
+        <v>441</v>
+      </c>
+      <c r="J1084" t="n">
+        <v>83</v>
+      </c>
+      <c r="K1084" t="n">
+        <v>107</v>
+      </c>
+      <c r="L1084" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1084" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>2025-12-11 11:02:40</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>11:02:40</t>
+        </is>
+      </c>
+      <c r="D1085" t="n">
+        <v>5762</v>
+      </c>
+      <c r="E1085" t="n">
+        <v>1161</v>
+      </c>
+      <c r="F1085" t="n">
+        <v>3918</v>
+      </c>
+      <c r="G1085" t="n">
+        <v>683</v>
+      </c>
+      <c r="H1085" t="n">
+        <v>180</v>
+      </c>
+      <c r="I1085" t="n">
+        <v>439</v>
+      </c>
+      <c r="J1085" t="n">
+        <v>84</v>
+      </c>
+      <c r="K1085" t="n">
+        <v>109</v>
+      </c>
+      <c r="L1085" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1085" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>2025-12-11 11:02:50</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>11:02:50</t>
+        </is>
+      </c>
+      <c r="D1086" t="n">
+        <v>5761</v>
+      </c>
+      <c r="E1086" t="n">
+        <v>1151</v>
+      </c>
+      <c r="F1086" t="n">
+        <v>3921</v>
+      </c>
+      <c r="G1086" t="n">
+        <v>689</v>
+      </c>
+      <c r="H1086" t="n">
+        <v>178</v>
+      </c>
+      <c r="I1086" t="n">
+        <v>442</v>
+      </c>
+      <c r="J1086" t="n">
+        <v>84</v>
+      </c>
+      <c r="K1086" t="n">
+        <v>111</v>
+      </c>
+      <c r="L1086" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1086" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>2025-12-11 11:03:00</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>11:03:00</t>
+        </is>
+      </c>
+      <c r="D1087" t="n">
+        <v>5766</v>
+      </c>
+      <c r="E1087" t="n">
+        <v>1152</v>
+      </c>
+      <c r="F1087" t="n">
+        <v>3918</v>
+      </c>
+      <c r="G1087" t="n">
+        <v>696</v>
+      </c>
+      <c r="H1087" t="n">
+        <v>179</v>
+      </c>
+      <c r="I1087" t="n">
+        <v>440</v>
+      </c>
+      <c r="J1087" t="n">
+        <v>84</v>
+      </c>
+      <c r="K1087" t="n">
+        <v>109</v>
+      </c>
+      <c r="L1087" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1087" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>2025-12-11 11:03:10</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>11:03:10</t>
+        </is>
+      </c>
+      <c r="D1088" t="n">
+        <v>5763</v>
+      </c>
+      <c r="E1088" t="n">
+        <v>1151</v>
+      </c>
+      <c r="F1088" t="n">
+        <v>3923</v>
+      </c>
+      <c r="G1088" t="n">
+        <v>689</v>
+      </c>
+      <c r="H1088" t="n">
+        <v>181</v>
+      </c>
+      <c r="I1088" t="n">
+        <v>446</v>
+      </c>
+      <c r="J1088" t="n">
+        <v>83</v>
+      </c>
+      <c r="K1088" t="n">
+        <v>112</v>
+      </c>
+      <c r="L1088" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1088" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>2025-12-11 11:03:20</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>11:03:20</t>
+        </is>
+      </c>
+      <c r="D1089" t="n">
+        <v>5765</v>
+      </c>
+      <c r="E1089" t="n">
+        <v>1147</v>
+      </c>
+      <c r="F1089" t="n">
+        <v>3927</v>
+      </c>
+      <c r="G1089" t="n">
+        <v>691</v>
+      </c>
+      <c r="H1089" t="n">
+        <v>180</v>
+      </c>
+      <c r="I1089" t="n">
+        <v>444</v>
+      </c>
+      <c r="J1089" t="n">
+        <v>85</v>
+      </c>
+      <c r="K1089" t="n">
+        <v>113</v>
+      </c>
+      <c r="L1089" t="n">
+        <v>35</v>
+      </c>
+      <c r="M1089" t="n">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>